<commit_message>
Atualizações do plano de acao
</commit_message>
<xml_diff>
--- a/Plano de Ação .xlsx
+++ b/Plano de Ação .xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\EcoYield\Documentos Organizacional\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\dinamica_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ED8B4F8-154E-41E9-BA7E-12CB05830192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4815A9A-759E-442B-AFA0-B8DDB907DC7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F06A637-B259-457E-B777-57329A3DB9A6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Tarefa</t>
   </si>
@@ -98,16 +98,16 @@
     <t>Kaue</t>
   </si>
   <si>
-    <t>Criação do Site por código</t>
-  </si>
-  <si>
-    <t>A Fazer</t>
-  </si>
-  <si>
     <t>Verificação do código de arduino</t>
   </si>
   <si>
     <t>Cristhian e Kaue</t>
+  </si>
+  <si>
+    <t>Script Banco de Dados</t>
+  </si>
+  <si>
+    <t>Feito</t>
   </si>
 </sst>
 </file>
@@ -168,7 +168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -181,6 +181,8 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="9" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,7 +601,7 @@
   <dimension ref="C3:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" zoomScale="114" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -681,7 +683,9 @@
       <c r="G7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="8">
+        <v>0.5</v>
+      </c>
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="3:9" x14ac:dyDescent="0.25">
@@ -700,7 +704,9 @@
       <c r="G8" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="9">
+        <v>0.7</v>
+      </c>
       <c r="I8" s="2"/>
     </row>
     <row r="9" spans="3:9" x14ac:dyDescent="0.25">
@@ -711,15 +717,17 @@
         <v>11</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F9" s="6">
         <v>45394</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="1"/>
+        <v>21</v>
+      </c>
+      <c r="H9" s="8">
+        <v>1</v>
+      </c>
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="3:9" x14ac:dyDescent="0.25">
@@ -738,7 +746,9 @@
       <c r="G10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="9">
+        <v>0.3</v>
+      </c>
       <c r="I10" s="2"/>
     </row>
     <row r="11" spans="3:9" x14ac:dyDescent="0.25">
@@ -757,12 +767,14 @@
       <c r="G11" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="8">
+        <v>0</v>
+      </c>
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>11</v>
@@ -774,26 +786,32 @@
         <v>45394</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1</v>
+      </c>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C13" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F13" s="6">
-        <v>45398</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
+        <v>45394</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="8">
+        <v>1</v>
+      </c>
       <c r="I13" s="1"/>
     </row>
     <row r="14" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>